<commit_message>
Report and Location Analysis
</commit_message>
<xml_diff>
--- a/Results 9 24 20.xlsx
+++ b/Results 9 24 20.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b544a48d06a5ece/UofL/Fall 2020/CSE 611/Homework/HW4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{9C57BC46-47DE-4CD6-B6B3-FC990A573026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32B2F172-5D01-4357-AF9D-2FD07442A727}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{9C57BC46-47DE-4CD6-B6B3-FC990A573026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9CF5B410-5FF8-42BE-9B98-2FCDFE43EAFB}"/>
   <bookViews>
-    <workbookView xWindow="22590" yWindow="3195" windowWidth="20490" windowHeight="16515" xr2:uid="{6723636D-5925-46EB-AA5C-6B0780D2804F}"/>
+    <workbookView xWindow="29205" yWindow="2220" windowWidth="20490" windowHeight="16515" xr2:uid="{6723636D-5925-46EB-AA5C-6B0780D2804F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>IJK</t>
   </si>
@@ -61,6 +63,9 @@
   </si>
   <si>
     <t>Latency (min)</t>
+  </si>
+  <si>
+    <t>Place</t>
   </si>
 </sst>
 </file>
@@ -92,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,13 +105,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,199 +146,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="147624704"/>
-        <c:axId val="146756000"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="147624704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="146756000"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="146756000"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="147624704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -417,22 +245,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>JKI</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KJI</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>IJK</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>JIK</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>IKJ</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>JIK</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>JKI</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>KIJ</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>KJI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -444,22 +272,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6.8204000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3132833333333345</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>12.107866666666666</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>14.258583333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>17.127716666666668</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.258583333333332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8204000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>17.359983333333332</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.3132833333333345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,46 +510,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1225,547 +1013,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2109694E-CECC-46A1-A050-DF91ECA26A94}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1796,7 +1045,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2102,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA951C0F-43AF-420F-AED8-6C9773802467}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,7 +1364,7 @@
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2125,80 +1374,113 @@
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>409.22399999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/60</f>
+        <v>6.8204000000000002</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>558.79700000000003</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3/60</f>
+        <v>9.3132833333333345</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="2">
         <v>726.47199999999998</v>
       </c>
-      <c r="C2">
-        <f>B2/60</f>
+      <c r="C4" s="2">
+        <f>B4/60</f>
         <v>12.107866666666666</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>855.51499999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5/60</f>
+        <v>14.258583333333332</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B6" s="2">
         <v>1027.663</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C7" si="0">B3/60</f>
+      <c r="C6" s="2">
+        <f>B6/60</f>
         <v>17.127716666666668</v>
       </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>855.51499999999999</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>14.258583333333332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>409.22399999999999</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>6.8204000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="2">
         <v>1041.5989999999999</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
+      <c r="C7" s="2">
+        <f>B7/60</f>
         <v>17.359983333333332</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>558.79700000000003</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>9.3132833333333345</v>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{259EA2CA-9A8F-4BD3-ABDF-18542E8CC9C8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E7">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>